<commit_message>
add next day to data
</commit_message>
<xml_diff>
--- a/history/25_35/data_ticker_1603.xlsx
+++ b/history/25_35/data_ticker_1603.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pavel.rostov\PycharmProjects\scrapyBotTrade\history\25_35\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1879356D-30F9-44DF-9742-5AA8E6B5893E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB46E59-E7B8-4369-971A-5C6A29ABF072}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1984,15 +1984,7 @@
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Процентный" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2DCDB"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -2333,11 +2325,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:CR252"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="CN144" sqref="CN144"/>
+      <selection activeCell="CM50" sqref="CM50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -2381,7 +2372,7 @@
       </c>
       <c r="I1" s="7">
         <f>H1/$E$2</f>
-        <v>2.8571428571428572</v>
+        <v>0.15503875968992248</v>
       </c>
     </row>
     <row r="2" spans="1:96" x14ac:dyDescent="0.25">
@@ -2391,7 +2382,7 @@
       <c r="C2" s="20"/>
       <c r="E2">
         <f>SUBTOTAL(  2,A:A)</f>
-        <v>7</v>
+        <v>129</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>587</v>
@@ -2401,14 +2392,14 @@
       </c>
       <c r="I2" s="7">
         <f t="shared" ref="I2:I6" si="0">H2/$E$2</f>
-        <v>1.1428571428571428</v>
+        <v>6.2015503875968991E-2</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>588</v>
       </c>
       <c r="L2" s="5">
         <f>SUBTOTAL( 9,CL:CL)</f>
-        <v>235.53999999999996</v>
+        <v>3990.85</v>
       </c>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
@@ -2420,14 +2411,14 @@
       </c>
       <c r="I3" s="7">
         <f t="shared" si="0"/>
-        <v>2.4285714285714284</v>
+        <v>0.13178294573643412</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>590</v>
       </c>
       <c r="L3" s="10">
         <f>SUBTOTAL( 9,CR:CR)</f>
-        <v>249.12647823190122</v>
+        <v>4040.4929945553527</v>
       </c>
     </row>
     <row r="4" spans="1:96" x14ac:dyDescent="0.25">
@@ -2439,14 +2430,14 @@
       </c>
       <c r="I4" s="7">
         <f t="shared" si="0"/>
-        <v>2.8571428571428572</v>
+        <v>0.15503875968992248</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>592</v>
       </c>
       <c r="L4" s="12">
         <f>100%-(L2/L3)</f>
-        <v>5.4536468095752522E-2</v>
+        <v>1.2286370653840417E-2</v>
       </c>
     </row>
     <row r="5" spans="1:96" x14ac:dyDescent="0.25">
@@ -2458,7 +2449,7 @@
       </c>
       <c r="I5" s="7">
         <f t="shared" si="0"/>
-        <v>4.1428571428571432</v>
+        <v>0.22480620155038761</v>
       </c>
     </row>
     <row r="6" spans="1:96" x14ac:dyDescent="0.25">
@@ -2470,7 +2461,7 @@
       </c>
       <c r="I6" s="7">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>0.27131782945736432</v>
       </c>
     </row>
     <row r="8" spans="1:96" x14ac:dyDescent="0.25">
@@ -2757,7 +2748,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="9" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -3047,7 +3038,7 @@
         <v>30.75</v>
       </c>
     </row>
-    <row r="10" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -3337,7 +3328,7 @@
         <v>30.52</v>
       </c>
     </row>
-    <row r="11" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -3627,7 +3618,7 @@
         <v>29.329127173542446</v>
       </c>
     </row>
-    <row r="12" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -3917,7 +3908,7 @@
         <v>30.116600265604252</v>
       </c>
     </row>
-    <row r="13" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -4207,7 +4198,7 @@
         <v>28.62</v>
       </c>
     </row>
-    <row r="14" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5</v>
       </c>
@@ -4497,7 +4488,7 @@
         <v>36.297688497523396</v>
       </c>
     </row>
-    <row r="15" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6</v>
       </c>
@@ -4787,7 +4778,7 @@
         <v>30.968834355828221</v>
       </c>
     </row>
-    <row r="16" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>7</v>
       </c>
@@ -5077,7 +5068,7 @@
         <v>34.19</v>
       </c>
     </row>
-    <row r="17" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>8</v>
       </c>
@@ -5367,7 +5358,7 @@
         <v>26.883439940498327</v>
       </c>
     </row>
-    <row r="18" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>9</v>
       </c>
@@ -5657,7 +5648,7 @@
         <v>28.449574692442884</v>
       </c>
     </row>
-    <row r="19" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10</v>
       </c>
@@ -5947,7 +5938,7 @@
         <v>27.02</v>
       </c>
     </row>
-    <row r="20" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>11</v>
       </c>
@@ -6237,7 +6228,7 @@
         <v>36.089600997506238</v>
       </c>
     </row>
-    <row r="21" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>12</v>
       </c>
@@ -6527,7 +6518,7 @@
         <v>34.224598305579896</v>
       </c>
     </row>
-    <row r="22" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>13</v>
       </c>
@@ -6817,7 +6808,7 @@
         <v>32.289393000929081</v>
       </c>
     </row>
-    <row r="23" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>14</v>
       </c>
@@ -7107,7 +7098,7 @@
         <v>32.159950248756218</v>
       </c>
     </row>
-    <row r="24" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>15</v>
       </c>
@@ -7397,7 +7388,7 @@
         <v>34.326827847363823</v>
       </c>
     </row>
-    <row r="25" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>16</v>
       </c>
@@ -7687,7 +7678,7 @@
         <v>31.929987472596302</v>
       </c>
     </row>
-    <row r="26" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>17</v>
       </c>
@@ -7977,7 +7968,7 @@
         <v>27.425534086766312</v>
       </c>
     </row>
-    <row r="27" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>18</v>
       </c>
@@ -8557,7 +8548,7 @@
         <v>35.908752431230901</v>
       </c>
     </row>
-    <row r="29" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>20</v>
       </c>
@@ -8847,7 +8838,7 @@
         <v>35.269656932237034</v>
       </c>
     </row>
-    <row r="30" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>21</v>
       </c>
@@ -9137,7 +9128,7 @@
         <v>27.493887272727271</v>
       </c>
     </row>
-    <row r="31" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>22</v>
       </c>
@@ -9427,7 +9418,7 @@
         <v>27.968569896317479</v>
       </c>
     </row>
-    <row r="32" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>23</v>
       </c>
@@ -9717,7 +9708,7 @@
         <v>25.79</v>
       </c>
     </row>
-    <row r="33" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>24</v>
       </c>
@@ -10007,7 +9998,7 @@
         <v>32.31693164243736</v>
       </c>
     </row>
-    <row r="34" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>25</v>
       </c>
@@ -10297,7 +10288,7 @@
         <v>25.97</v>
       </c>
     </row>
-    <row r="35" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>26</v>
       </c>
@@ -10587,7 +10578,7 @@
         <v>33.33</v>
       </c>
     </row>
-    <row r="36" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>27</v>
       </c>
@@ -10877,7 +10868,7 @@
         <v>33.236919374247897</v>
       </c>
     </row>
-    <row r="37" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>28</v>
       </c>
@@ -11167,7 +11158,7 @@
         <v>32.46</v>
       </c>
     </row>
-    <row r="38" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>29</v>
       </c>
@@ -11457,7 +11448,7 @@
         <v>33.159999999999997</v>
       </c>
     </row>
-    <row r="39" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>30</v>
       </c>
@@ -11747,7 +11738,7 @@
         <v>33.51694510739857</v>
       </c>
     </row>
-    <row r="40" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>31</v>
       </c>
@@ -12037,7 +12028,7 @@
         <v>33.229999999999997</v>
       </c>
     </row>
-    <row r="41" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>32</v>
       </c>
@@ -12327,7 +12318,7 @@
         <v>34.326934412019646</v>
       </c>
     </row>
-    <row r="42" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>33</v>
       </c>
@@ -12617,7 +12608,7 @@
         <v>30.846029173419772</v>
       </c>
     </row>
-    <row r="43" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>34</v>
       </c>
@@ -12907,7 +12898,7 @@
         <v>28.164070262597587</v>
       </c>
     </row>
-    <row r="44" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>35</v>
       </c>
@@ -13197,7 +13188,7 @@
         <v>27.096678966789671</v>
       </c>
     </row>
-    <row r="45" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>36</v>
       </c>
@@ -13487,7 +13478,7 @@
         <v>32.401711906230723</v>
       </c>
     </row>
-    <row r="46" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>37</v>
       </c>
@@ -13777,7 +13768,7 @@
         <v>29.116699862637365</v>
       </c>
     </row>
-    <row r="47" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>38</v>
       </c>
@@ -14067,7 +14058,7 @@
         <v>29.598648648648648</v>
       </c>
     </row>
-    <row r="48" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>39</v>
       </c>
@@ -14357,7 +14348,7 @@
         <v>27.709967520750631</v>
       </c>
     </row>
-    <row r="49" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>40</v>
       </c>
@@ -14937,7 +14928,7 @@
         <v>34.200000000000003</v>
       </c>
     </row>
-    <row r="51" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>42</v>
       </c>
@@ -15227,7 +15218,7 @@
         <v>33.017952755905519</v>
       </c>
     </row>
-    <row r="52" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>43</v>
       </c>
@@ -15517,7 +15508,7 @@
         <v>38.987349397590357</v>
       </c>
     </row>
-    <row r="53" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>44</v>
       </c>
@@ -15807,7 +15798,7 @@
         <v>28.956191790272506</v>
       </c>
     </row>
-    <row r="54" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>45</v>
       </c>
@@ -16097,7 +16088,7 @@
         <v>32.483159188690841</v>
       </c>
     </row>
-    <row r="55" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>46</v>
       </c>
@@ -16387,7 +16378,7 @@
         <v>27.18</v>
       </c>
     </row>
-    <row r="56" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>47</v>
       </c>
@@ -16677,7 +16668,7 @@
         <v>30.95</v>
       </c>
     </row>
-    <row r="57" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>48</v>
       </c>
@@ -16967,7 +16958,7 @@
         <v>29.979969979986659</v>
       </c>
     </row>
-    <row r="58" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>49</v>
       </c>
@@ -17257,7 +17248,7 @@
         <v>31.56</v>
       </c>
     </row>
-    <row r="59" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>50</v>
       </c>
@@ -17547,7 +17538,7 @@
         <v>29.64486513823331</v>
       </c>
     </row>
-    <row r="60" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>51</v>
       </c>
@@ -17837,7 +17828,7 @@
         <v>35.32</v>
       </c>
     </row>
-    <row r="61" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>52</v>
       </c>
@@ -18417,7 +18408,7 @@
         <v>37.608499335989372</v>
       </c>
     </row>
-    <row r="63" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>54</v>
       </c>
@@ -18707,7 +18698,7 @@
         <v>31.28</v>
       </c>
     </row>
-    <row r="64" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>55</v>
       </c>
@@ -18997,7 +18988,7 @@
         <v>28.418138634764251</v>
       </c>
     </row>
-    <row r="65" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>56</v>
       </c>
@@ -19287,7 +19278,7 @@
         <v>26.819966442953021</v>
       </c>
     </row>
-    <row r="66" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>57</v>
       </c>
@@ -19867,7 +19858,7 @@
         <v>44.906530048842647</v>
       </c>
     </row>
-    <row r="68" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>59</v>
       </c>
@@ -20157,7 +20148,7 @@
         <v>32.159999999999997</v>
       </c>
     </row>
-    <row r="69" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>60</v>
       </c>
@@ -20447,7 +20438,7 @@
         <v>28.83</v>
       </c>
     </row>
-    <row r="70" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>61</v>
       </c>
@@ -20737,7 +20728,7 @@
         <v>27.989967857142858</v>
       </c>
     </row>
-    <row r="71" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>62</v>
       </c>
@@ -21027,7 +21018,7 @@
         <v>26.219538520213575</v>
       </c>
     </row>
-    <row r="72" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>63</v>
       </c>
@@ -21317,7 +21308,7 @@
         <v>25.909243535314552</v>
       </c>
     </row>
-    <row r="73" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>64</v>
       </c>
@@ -21607,7 +21598,7 @@
         <v>32.005248359887531</v>
       </c>
     </row>
-    <row r="74" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>65</v>
       </c>
@@ -21897,7 +21888,7 @@
         <v>38.43854691967767</v>
       </c>
     </row>
-    <row r="75" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>66</v>
       </c>
@@ -22187,7 +22178,7 @@
         <v>30.299257425742578</v>
       </c>
     </row>
-    <row r="76" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>67</v>
       </c>
@@ -22477,7 +22468,7 @@
         <v>32.469479519556515</v>
       </c>
     </row>
-    <row r="77" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>68</v>
       </c>
@@ -22767,7 +22758,7 @@
         <v>31.958044430538173</v>
       </c>
     </row>
-    <row r="78" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>69</v>
       </c>
@@ -23057,7 +23048,7 @@
         <v>36.698013623978206</v>
       </c>
     </row>
-    <row r="79" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>70</v>
       </c>
@@ -23347,7 +23338,7 @@
         <v>33.92870026525199</v>
       </c>
     </row>
-    <row r="80" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>71</v>
       </c>
@@ -23637,7 +23628,7 @@
         <v>25.27</v>
       </c>
     </row>
-    <row r="81" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>72</v>
       </c>
@@ -23927,7 +23918,7 @@
         <v>32.383467119481324</v>
       </c>
     </row>
-    <row r="82" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>73</v>
       </c>
@@ -24217,7 +24208,7 @@
         <v>35.877499999999998</v>
       </c>
     </row>
-    <row r="83" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>74</v>
       </c>
@@ -24507,7 +24498,7 @@
         <v>29.887908999665441</v>
       </c>
     </row>
-    <row r="84" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>75</v>
       </c>
@@ -24797,7 +24788,7 @@
         <v>34.957757437070939</v>
       </c>
     </row>
-    <row r="85" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>76</v>
       </c>
@@ -25087,7 +25078,7 @@
         <v>33.289411234604984</v>
       </c>
     </row>
-    <row r="86" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>77</v>
       </c>
@@ -25377,7 +25368,7 @@
         <v>27.749996396396398</v>
       </c>
     </row>
-    <row r="87" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>78</v>
       </c>
@@ -25667,7 +25658,7 @@
         <v>32.749218320610687</v>
       </c>
     </row>
-    <row r="88" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>79</v>
       </c>
@@ -25957,7 +25948,7 @@
         <v>34.429648562300315</v>
       </c>
     </row>
-    <row r="89" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>80</v>
       </c>
@@ -26247,7 +26238,7 @@
         <v>35.76637685211071</v>
       </c>
     </row>
-    <row r="90" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>81</v>
       </c>
@@ -26537,7 +26528,7 @@
         <v>33.176094032549727</v>
       </c>
     </row>
-    <row r="91" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>82</v>
       </c>
@@ -26827,7 +26818,7 @@
         <v>31.888617121354656</v>
       </c>
     </row>
-    <row r="92" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>83</v>
       </c>
@@ -27117,7 +27108,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="93" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>84</v>
       </c>
@@ -27407,7 +27398,7 @@
         <v>33.715489323843414</v>
       </c>
     </row>
-    <row r="94" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>85</v>
       </c>
@@ -27697,7 +27688,7 @@
         <v>31.339987236758137</v>
       </c>
     </row>
-    <row r="95" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>86</v>
       </c>
@@ -27987,7 +27978,7 @@
         <v>30.19</v>
       </c>
     </row>
-    <row r="96" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>87</v>
       </c>
@@ -28277,7 +28268,7 @@
         <v>28.18</v>
       </c>
     </row>
-    <row r="97" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>88</v>
       </c>
@@ -28567,7 +28558,7 @@
         <v>35.22</v>
       </c>
     </row>
-    <row r="98" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>89</v>
       </c>
@@ -28857,7 +28848,7 @@
         <v>26.26</v>
       </c>
     </row>
-    <row r="99" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>90</v>
       </c>
@@ -29147,7 +29138,7 @@
         <v>32.819402803168799</v>
       </c>
     </row>
-    <row r="100" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>91</v>
       </c>
@@ -29437,7 +29428,7 @@
         <v>28.7</v>
       </c>
     </row>
-    <row r="101" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>92</v>
       </c>
@@ -29727,7 +29718,7 @@
         <v>29.509945781091158</v>
       </c>
     </row>
-    <row r="102" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>93</v>
       </c>
@@ -30017,7 +30008,7 @@
         <v>28.669996512033485</v>
       </c>
     </row>
-    <row r="103" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>94</v>
       </c>
@@ -30307,7 +30298,7 @@
         <v>30.909171789065027</v>
       </c>
     </row>
-    <row r="104" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>95</v>
       </c>
@@ -30597,7 +30588,7 @@
         <v>35.944378648874057</v>
       </c>
     </row>
-    <row r="105" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>96</v>
       </c>
@@ -30887,7 +30878,7 @@
         <v>31.9758</v>
       </c>
     </row>
-    <row r="106" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>97</v>
       </c>
@@ -31177,7 +31168,7 @@
         <v>26.25</v>
       </c>
     </row>
-    <row r="107" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>98</v>
       </c>
@@ -31467,7 +31458,7 @@
         <v>35.65</v>
       </c>
     </row>
-    <row r="108" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>99</v>
       </c>
@@ -31757,7 +31748,7 @@
         <v>27.48417970170971</v>
       </c>
     </row>
-    <row r="109" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>100</v>
       </c>
@@ -32047,7 +32038,7 @@
         <v>31.6</v>
       </c>
     </row>
-    <row r="110" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>101</v>
       </c>
@@ -32627,7 +32618,7 @@
         <v>28.749499130434781</v>
       </c>
     </row>
-    <row r="112" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>103</v>
       </c>
@@ -32917,7 +32908,7 @@
         <v>36.19889502762431</v>
       </c>
     </row>
-    <row r="113" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>104</v>
       </c>
@@ -33207,7 +33198,7 @@
         <v>29.61802267422474</v>
       </c>
     </row>
-    <row r="114" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>105</v>
       </c>
@@ -33497,7 +33488,7 @@
         <v>27.56982227058397</v>
       </c>
     </row>
-    <row r="115" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>106</v>
       </c>
@@ -33787,7 +33778,7 @@
         <v>31.58</v>
       </c>
     </row>
-    <row r="116" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>107</v>
       </c>
@@ -34077,7 +34068,7 @@
         <v>31.009890393294651</v>
       </c>
     </row>
-    <row r="117" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>108</v>
       </c>
@@ -34657,7 +34648,7 @@
         <v>34.741294964028775</v>
       </c>
     </row>
-    <row r="119" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>110</v>
       </c>
@@ -34947,7 +34938,7 @@
         <v>37.825651254953762</v>
       </c>
     </row>
-    <row r="120" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>111</v>
       </c>
@@ -35237,7 +35228,7 @@
         <v>28.199202127659571</v>
       </c>
     </row>
-    <row r="121" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>112</v>
       </c>
@@ -35527,7 +35518,7 @@
         <v>29.43</v>
       </c>
     </row>
-    <row r="122" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>113</v>
       </c>
@@ -35817,7 +35808,7 @@
         <v>27.766078501980552</v>
       </c>
     </row>
-    <row r="123" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>114</v>
       </c>
@@ -36397,7 +36388,7 @@
         <v>33.011902321374734</v>
       </c>
     </row>
-    <row r="125" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>116</v>
       </c>
@@ -36687,7 +36678,7 @@
         <v>33.15646668676515</v>
       </c>
     </row>
-    <row r="126" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>117</v>
       </c>
@@ -36977,7 +36968,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="127" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>118</v>
       </c>
@@ -37267,7 +37258,7 @@
         <v>30.01</v>
       </c>
     </row>
-    <row r="128" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>119</v>
       </c>
@@ -37557,7 +37548,7 @@
         <v>26.169904470768056</v>
       </c>
     </row>
-    <row r="129" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>120</v>
       </c>
@@ -37847,7 +37838,7 @@
         <v>26.679696401799102</v>
       </c>
     </row>
-    <row r="130" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>121</v>
       </c>
@@ -38137,7 +38128,7 @@
         <v>33.029987889797155</v>
       </c>
     </row>
-    <row r="131" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>122</v>
       </c>
@@ -38427,7 +38418,7 @@
         <v>34.977925121463272</v>
       </c>
     </row>
-    <row r="132" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>123</v>
       </c>
@@ -38717,7 +38708,7 @@
         <v>26.75</v>
       </c>
     </row>
-    <row r="133" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>124</v>
       </c>
@@ -39007,7 +38998,7 @@
         <v>26.227983225314528</v>
       </c>
     </row>
-    <row r="134" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>125</v>
       </c>
@@ -39297,7 +39288,7 @@
         <v>32.48855076923077</v>
       </c>
     </row>
-    <row r="135" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>126</v>
       </c>
@@ -39587,7 +39578,7 @@
         <v>37.499733333333332</v>
       </c>
     </row>
-    <row r="136" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>127</v>
       </c>
@@ -39877,7 +39868,7 @@
         <v>31.07997104247104</v>
       </c>
     </row>
-    <row r="137" spans="1:96" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>128</v>
       </c>
@@ -40858,42 +40849,38 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A8:CP137" xr:uid="{71C3FF4A-7E9A-4F5A-A14E-FAA416DCFD06}">
-    <filterColumn colId="1">
-      <colorFilter dxfId="0"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A8:CP137" xr:uid="{71C3FF4A-7E9A-4F5A-A14E-FAA416DCFD06}"/>
   <mergeCells count="1">
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <conditionalFormatting sqref="CP9:CP137">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="between">
       <formula>1%</formula>
       <formula>1.5%</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CP9:CP137">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="between">
       <formula>0.015</formula>
       <formula>0.02</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CP9:CP137">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>0.02</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CP9:CP137">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
       <formula>0.005</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="between">
       <formula>0.005</formula>
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CP9:CP137">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>